<commit_message>
export database to excel
</commit_message>
<xml_diff>
--- a/customer.xlsx
+++ b/customer.xlsx
@@ -11,39 +11,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Id</t>
   </si>
   <si>
+    <t>createdAt</t>
+  </si>
+  <si>
+    <t>idAgency</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>entryPrice</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>fee</t>
+  </si>
+  <si>
+    <t>agencySupport</t>
+  </si>
+  <si>
+    <t>feeIfFalse</t>
+  </si>
+  <si>
     <t>Status</t>
   </si>
   <si>
-    <t>Sim</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
     <t>"5efaeade23aead2ee498a509"</t>
   </si>
   <si>
+    <t>5ef416418403f41103f35edd</t>
+  </si>
+  <si>
+    <t>011111111</t>
+  </si>
+  <si>
     <t>success</t>
   </si>
   <si>
-    <t>011111111</t>
-  </si>
-  <si>
     <t>"5efaeae523aead2ee498a50a"</t>
   </si>
   <si>
+    <t>5ef416468403f41103f35ede</t>
+  </si>
+  <si>
     <t>0123456789</t>
   </si>
   <si>
     <t>"5efaeae923aead2ee498a50b"</t>
   </si>
   <si>
+    <t>5ef46fa44cd9972ca7256f6d</t>
+  </si>
+  <si>
     <t>"5efaeaed23aead2ee498a50c"</t>
+  </si>
+  <si>
+    <t>5ef95562754fbb138d45b48b</t>
   </si>
   <si>
     <t>"5efc3a42c7471527b4d171ae"</t>
@@ -91,8 +121,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,15 +463,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:J7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="2" width="50" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="10" outlineLevel="1" collapsed="1" customWidth="1"/>
+    <col min="1" max="1" width="50" customWidth="1"/>
+    <col min="2" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,71 +483,215 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44012.31517321759</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>1000000</v>
+      </c>
+      <c r="F2">
+        <v>1500000</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44012.315246122685</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>1000000</v>
+      </c>
+      <c r="F3">
+        <v>1500000</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44012.31529115741</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>1000000</v>
+      </c>
+      <c r="F4">
+        <v>1500000</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44012.315336238426</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>1000000</v>
+      </c>
+      <c r="F5">
+        <v>1500000</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44013.30892015046</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>1354</v>
+      </c>
+      <c r="F6">
+        <v>5154125</v>
+      </c>
+      <c r="G6">
+        <v>1451245</v>
+      </c>
+      <c r="H6">
+        <v>154155</v>
+      </c>
+      <c r="I6">
+        <v>345435415</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44013.30956559027</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <v>3243</v>
+      </c>
+      <c r="F7">
+        <v>55245</v>
+      </c>
+      <c r="G7">
+        <v>245</v>
+      </c>
+      <c r="H7">
+        <v>5235325</v>
+      </c>
+      <c r="I7">
+        <v>5325235</v>
+      </c>
+      <c r="J7" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>